<commit_message>
make field build script systematic and consistent naming convention
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Development/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4653144F-35DF-514B-93EB-218EED11B05C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C98ADE2-BEC8-694F-933C-F6D1AD9EDDC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17300" yWindow="3960" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="6020" yWindow="4020" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
     <t>field</t>
   </si>
   <si>
-    <t>activityType</t>
-  </si>
-  <si>
     <t>MinHeartRate</t>
   </si>
   <si>
@@ -360,12 +357,15 @@
   </si>
   <si>
     <t>Threshold Power</t>
+  </si>
+  <si>
+    <t>activity_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1199,10 +1199,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
@@ -1217,415 +1217,415 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
         <v>30</v>
-      </c>
-      <c r="B39" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
         <v>30</v>
-      </c>
-      <c r="B41" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1635,11 +1635,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1654,629 +1654,629 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
         <v>101</v>
-      </c>
-      <c r="D1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
step toward better diff and not missing fields
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Development/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C98ADE2-BEC8-694F-933C-F6D1AD9EDDC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75680A0C-AB23-C34A-B7C3-1E02923155AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="4020" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="4460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="166">
   <si>
     <t>field</t>
   </si>
@@ -360,6 +360,165 @@
   </si>
   <si>
     <t>activity_type</t>
+  </si>
+  <si>
+    <t>GainCorrectedElevation</t>
+  </si>
+  <si>
+    <t>GainUncorrectedElevation</t>
+  </si>
+  <si>
+    <t>LossCorrectedElevation</t>
+  </si>
+  <si>
+    <t>LossUncorrectedElevation</t>
+  </si>
+  <si>
+    <t>MaxCorrectedElevation</t>
+  </si>
+  <si>
+    <t>MaxGroundContactTime</t>
+  </si>
+  <si>
+    <t>MaxMomentaryEnergyExpenditure</t>
+  </si>
+  <si>
+    <t>MaxRelativeRunningEconomy</t>
+  </si>
+  <si>
+    <t>MaxUncorrectedElevation</t>
+  </si>
+  <si>
+    <t>MaxVerticalOscillation</t>
+  </si>
+  <si>
+    <t>MaxVerticalSpeed</t>
+  </si>
+  <si>
+    <t>MinBikeCadence</t>
+  </si>
+  <si>
+    <t>MinCorrectedElevation</t>
+  </si>
+  <si>
+    <t>MinGroundContactTime</t>
+  </si>
+  <si>
+    <t>MinMomentaryEnergyExpenditure</t>
+  </si>
+  <si>
+    <t>MinPace</t>
+  </si>
+  <si>
+    <t>MinRelativeRunningEconomy</t>
+  </si>
+  <si>
+    <t>MinRunCadence</t>
+  </si>
+  <si>
+    <t>MinUncorrectedElevation</t>
+  </si>
+  <si>
+    <t>MinVerticalOscillation</t>
+  </si>
+  <si>
+    <t>SumAnaerobicTrainingEffect</t>
+  </si>
+  <si>
+    <t>SumFloorsClimbed</t>
+  </si>
+  <si>
+    <t>SumFloorsDescended</t>
+  </si>
+  <si>
+    <t>WeightedMeanLeftBalance</t>
+  </si>
+  <si>
+    <t>WeightedMeanMomentaryEnergyExpenditure</t>
+  </si>
+  <si>
+    <t>WeightedMeanRelativeRunningEconomy</t>
+  </si>
+  <si>
+    <t>WeightedMeanStanceTime</t>
+  </si>
+  <si>
+    <t>WeightedMeanStanceTimePercent</t>
+  </si>
+  <si>
+    <t>WeightedMeanVerticalSpeed</t>
+  </si>
+  <si>
+    <t>Elevation Gain</t>
+  </si>
+  <si>
+    <t>Elevation Loss</t>
+  </si>
+  <si>
+    <t>Max Elevation</t>
+  </si>
+  <si>
+    <t>Max Ground Contact Time</t>
+  </si>
+  <si>
+    <t>Max Energy Expenditure</t>
+  </si>
+  <si>
+    <t>Max Running Economy</t>
+  </si>
+  <si>
+    <t>Max Vertical Oscillation</t>
+  </si>
+  <si>
+    <t>Max Vertical Speed</t>
+  </si>
+  <si>
+    <t>Min Cadence</t>
+  </si>
+  <si>
+    <t>Min Elevation</t>
+  </si>
+  <si>
+    <t>Min Ground Contact Time</t>
+  </si>
+  <si>
+    <t>Min Energy Expenditure</t>
+  </si>
+  <si>
+    <t>Min Pace</t>
+  </si>
+  <si>
+    <t>Min Running Economy</t>
+  </si>
+  <si>
+    <t>Min Vertical Oscillation</t>
+  </si>
+  <si>
+    <t>Anaerobic Training Effect</t>
+  </si>
+  <si>
+    <t>Floors Climbed</t>
+  </si>
+  <si>
+    <t>Floors Descended</t>
+  </si>
+  <si>
+    <t>Avg Left Balance</t>
+  </si>
+  <si>
+    <t>Avg Energy Expenditure</t>
+  </si>
+  <si>
+    <t>Avg Running Economy</t>
+  </si>
+  <si>
+    <t>Avg Stance Time</t>
+  </si>
+  <si>
+    <t>Avg Stance Percent</t>
+  </si>
+  <si>
+    <t>Avg Vertical Speed</t>
   </si>
 </sst>
 </file>
@@ -1200,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1628,6 +1787,238 @@
         <v>53</v>
       </c>
     </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>131</v>
+      </c>
+      <c r="B71" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>135</v>
+      </c>
+      <c r="B75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>139</v>
+      </c>
+      <c r="B79" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>141</v>
+      </c>
+      <c r="B81" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1638,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
rename best rolling to critical
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Development/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75680A0C-AB23-C34A-B7C3-1E02923155AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA4248-2EC9-2D41-A3B1-E33A2AD814C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="4460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11660" yWindow="1600" windowWidth="33340" windowHeight="24540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="178">
   <si>
     <t>field</t>
   </si>
@@ -519,13 +519,49 @@
   </si>
   <si>
     <t>Avg Vertical Speed</t>
+  </si>
+  <si>
+    <t>__CalcBestRollingWeightedMeanHeartRate</t>
+  </si>
+  <si>
+    <t>Critical Heart Rate</t>
+  </si>
+  <si>
+    <t>__CalcBestRollingWeightedMeanPower</t>
+  </si>
+  <si>
+    <t>Critical Power</t>
+  </si>
+  <si>
+    <t>__CalcBestRollingWeightedMeanSpeed</t>
+  </si>
+  <si>
+    <t>Critical Speed</t>
+  </si>
+  <si>
+    <t>__CalcBestRollingWeightedMeanPace</t>
+  </si>
+  <si>
+    <t>Critical Pace</t>
+  </si>
+  <si>
+    <t>kph</t>
+  </si>
+  <si>
+    <t>mph</t>
+  </si>
+  <si>
+    <t>minperkm</t>
+  </si>
+  <si>
+    <t>minpermile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1359,19 +1395,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:A85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1379,7 +1415,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +1431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1411,7 +1447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1419,7 +1455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1427,7 +1463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1435,7 +1471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1443,7 +1479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1451,7 +1487,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1459,7 +1495,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1467,7 +1503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1475,7 +1511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1483,7 +1519,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1491,7 +1527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1499,7 +1535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1507,7 +1543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1515,7 +1551,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1523,7 +1559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1531,7 +1567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1539,7 +1575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1547,7 +1583,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1555,7 +1591,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1563,7 +1599,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1571,7 +1607,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1579,7 +1615,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -1587,7 +1623,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1595,7 +1631,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -1603,7 +1639,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -1611,7 +1647,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -1619,7 +1655,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -1627,7 +1663,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -1635,7 +1671,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -1643,7 +1679,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -1651,7 +1687,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -1659,7 +1695,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -1667,7 +1703,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1675,7 +1711,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -1683,7 +1719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -1691,7 +1727,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1699,7 +1735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -1707,7 +1743,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -1715,7 +1751,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -1723,7 +1759,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1731,7 +1767,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -1739,7 +1775,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1747,7 +1783,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -1755,7 +1791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -1763,7 +1799,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1771,7 +1807,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1779,7 +1815,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -1787,7 +1823,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -1795,7 +1831,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -1803,7 +1839,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -1811,7 +1847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -1819,7 +1855,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -1827,7 +1863,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -1835,7 +1871,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -1843,7 +1879,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -1851,7 +1887,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -1859,7 +1895,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -1867,7 +1903,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -1875,7 +1911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -1883,7 +1919,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -1891,7 +1927,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -1899,7 +1935,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -1907,7 +1943,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -1915,7 +1951,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>129</v>
       </c>
@@ -1923,7 +1959,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -1931,7 +1967,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>131</v>
       </c>
@@ -1939,7 +1975,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>132</v>
       </c>
@@ -1947,7 +1983,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>133</v>
       </c>
@@ -1955,7 +1991,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>134</v>
       </c>
@@ -1963,7 +1999,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>135</v>
       </c>
@@ -1971,7 +2007,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>136</v>
       </c>
@@ -1979,7 +2015,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>137</v>
       </c>
@@ -1987,7 +2023,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>138</v>
       </c>
@@ -1995,7 +2031,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>139</v>
       </c>
@@ -2003,7 +2039,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>140</v>
       </c>
@@ -2011,12 +2047,44 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>141</v>
       </c>
       <c r="B81" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>166</v>
+      </c>
+      <c r="B82" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2027,20 +2095,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2122,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2065,10 +2133,10 @@
         <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2082,7 +2150,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -2096,7 +2164,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2110,7 +2178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2124,7 +2192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2138,7 +2206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2152,7 +2220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -2166,7 +2234,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -2180,7 +2248,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -2194,7 +2262,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2208,7 +2276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2222,7 +2290,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2236,7 +2304,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -2250,7 +2318,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -2264,7 +2332,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -2278,7 +2346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2292,7 +2360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2306,7 +2374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2320,7 +2388,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2334,7 +2402,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2348,7 +2416,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2362,7 +2430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2376,7 +2444,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2390,7 +2458,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2404,7 +2472,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -2418,7 +2486,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -2432,7 +2500,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2446,7 +2514,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -2460,7 +2528,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2474,7 +2542,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -2488,7 +2556,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2502,7 +2570,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -2516,7 +2584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2530,7 +2598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -2544,7 +2612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -2558,7 +2626,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -2572,7 +2640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -2586,7 +2654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2600,7 +2668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2614,7 +2682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2628,7 +2696,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -2642,7 +2710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -2656,7 +2724,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2668,6 +2736,62 @@
       </c>
       <c r="D45" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix name to be peak power
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Development/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA4248-2EC9-2D41-A3B1-E33A2AD814C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B94B6CE-AAA8-E046-BDF1-ECD16F694BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="1600" windowWidth="33340" windowHeight="24540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2500" yWindow="460" windowWidth="33340" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
@@ -524,27 +524,15 @@
     <t>__CalcBestRollingWeightedMeanHeartRate</t>
   </si>
   <si>
-    <t>Critical Heart Rate</t>
-  </si>
-  <si>
     <t>__CalcBestRollingWeightedMeanPower</t>
   </si>
   <si>
-    <t>Critical Power</t>
-  </si>
-  <si>
     <t>__CalcBestRollingWeightedMeanSpeed</t>
   </si>
   <si>
-    <t>Critical Speed</t>
-  </si>
-  <si>
     <t>__CalcBestRollingWeightedMeanPace</t>
   </si>
   <si>
-    <t>Critical Pace</t>
-  </si>
-  <si>
     <t>kph</t>
   </si>
   <si>
@@ -555,13 +543,25 @@
   </si>
   <si>
     <t>minpermile</t>
+  </si>
+  <si>
+    <t>Peak Heart Rate</t>
+  </si>
+  <si>
+    <t>Peak Power</t>
+  </si>
+  <si>
+    <t>Peak Speed</t>
+  </si>
+  <si>
+    <t>Peak Pace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1397,17 +1397,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:A85"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>129</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>131</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>132</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>133</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>134</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>135</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>136</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>137</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>138</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>139</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>140</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>141</v>
       </c>
@@ -2055,36 +2055,36 @@
         <v>165</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>166</v>
       </c>
       <c r="B82" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
+      <c r="B83" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>168</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>170</v>
-      </c>
-      <c r="B84" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>172</v>
-      </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2097,18 +2097,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>166</v>
       </c>
@@ -2752,9 +2752,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -2766,32 +2766,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D48" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
don't compound meters into kilometers for elevation
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Development/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B94B6CE-AAA8-E046-BDF1-ECD16F694BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88F665C-8174-FA4E-8DAD-9A373FCCFD9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="460" windowWidth="33340" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2500" yWindow="460" windowWidth="33340" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="185">
   <si>
     <t>field</t>
   </si>
@@ -555,6 +555,27 @@
   </si>
   <si>
     <t>Peak Pace</t>
+  </si>
+  <si>
+    <t>GainElevation</t>
+  </si>
+  <si>
+    <t>LossElevation</t>
+  </si>
+  <si>
+    <t>MaxElevation</t>
+  </si>
+  <si>
+    <t>MinElevation</t>
+  </si>
+  <si>
+    <t>SumSampleCountElevation</t>
+  </si>
+  <si>
+    <t>meterelevation</t>
+  </si>
+  <si>
+    <t>footelevation</t>
   </si>
 </sst>
 </file>
@@ -1397,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2095,10 +2116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2794,6 +2815,202 @@
         <v>173</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D50" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>183</v>
+      </c>
+      <c r="D52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>179</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>183</v>
+      </c>
+      <c r="D54" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>183</v>
+      </c>
+      <c r="D55" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>183</v>
+      </c>
+      <c r="D56" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>180</v>
+      </c>
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>183</v>
+      </c>
+      <c r="D58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>181</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>183</v>
+      </c>
+      <c r="D61" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>183</v>
+      </c>
+      <c r="D62" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D63" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
     <sortCondition ref="A2:A45"/>

</xml_diff>

<commit_message>
moved celsius to be the default
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Development/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88F665C-8174-FA4E-8DAD-9A373FCCFD9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBCBD78-2B9A-3B43-BBD9-3E13D4C411F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="460" windowWidth="33340" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2500" yWindow="500" windowWidth="33340" windowHeight="25880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="190">
   <si>
     <t>field</t>
   </si>
@@ -576,13 +576,28 @@
   </si>
   <si>
     <t>footelevation</t>
+  </si>
+  <si>
+    <t>MaxAirTemperature</t>
+  </si>
+  <si>
+    <t>fahrenheit</t>
+  </si>
+  <si>
+    <t>MinAirTemperature</t>
+  </si>
+  <si>
+    <t>WeightedMeanAirTemperature</t>
+  </si>
+  <si>
+    <t>celsius</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -713,6 +728,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1059,8 +1081,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2116,10 +2139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3011,6 +3034,48 @@
         <v>184</v>
       </c>
     </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
     <sortCondition ref="A2:A45"/>

</xml_diff>

<commit_message>
Initial Running Effectiveness missing units and weight scaling #98
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Development/public/connectstats/ConnectStats/sqlite/edit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBCBD78-2B9A-3B43-BBD9-3E13D4C411F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95A16B4-091F-E647-AAF1-296B0206F3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="500" windowWidth="33340" windowHeight="25880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="660" windowWidth="33340" windowHeight="25880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="192">
   <si>
     <t>field</t>
   </si>
@@ -591,6 +591,12 @@
   </si>
   <si>
     <t>celsius</t>
+  </si>
+  <si>
+    <t>__CalcRunningEffectiveness</t>
+  </si>
+  <si>
+    <t>Running Effectiveness</t>
   </si>
 </sst>
 </file>
@@ -1439,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2131,6 +2137,14 @@
         <v>177</v>
       </c>
     </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>190</v>
+      </c>
+      <c r="B86" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2139,10 +2153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3076,6 +3090,20 @@
         <v>186</v>
       </c>
     </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
     <sortCondition ref="A2:A45"/>

</xml_diff>

<commit_message>
fix up fields update and order for running effeciency #98
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
+++ b/ConnectStats/sqlite/edit/gc_fields_manual.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/connectstats/ConnectStats/sqlite/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95A16B4-091F-E647-AAF1-296B0206F3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2D4A02-8750-4442-A791-D9C2CCAF6535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="660" windowWidth="33340" windowHeight="25880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55760" yWindow="2240" windowWidth="33340" windowHeight="25880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gc_fields_display" sheetId="1" r:id="rId1"/>
     <sheet name="gc_fields_uom" sheetId="2" r:id="rId2"/>
+    <sheet name="gc_fields_order" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="196">
   <si>
     <t>field</t>
   </si>
@@ -597,6 +598,18 @@
   </si>
   <si>
     <t>Running Effectiveness</t>
+  </si>
+  <si>
+    <t>field_order</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>__CalcMetabolicEfficiency</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1461,7 @@
   <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2155,7 +2168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
@@ -3111,4 +3124,58 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932BD0AC-0BED-4949-8CF2-120B3544534F}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>